<commit_message>
Definición de mas servicios y ajuste de horas invertidas en el proyecto
</commit_message>
<xml_diff>
--- a/Definicion de servicios.xlsx
+++ b/Definicion de servicios.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>crearAlimento</t>
   </si>
@@ -84,6 +84,48 @@
   </si>
   <si>
     <t>codigoError, mensaje y listado de menus de alimento por objetos de cada uno de los solicitados.</t>
+  </si>
+  <si>
+    <t>crearUsuario</t>
+  </si>
+  <si>
+    <t>Este servicio debe permitir crear un usuario con los datos basicos</t>
+  </si>
+  <si>
+    <t>crearYAsignarHijo</t>
+  </si>
+  <si>
+    <t>Este servicio debe permitir crear un hijo y ser asignado a su respectivo padre</t>
+  </si>
+  <si>
+    <t>consultarHijos</t>
+  </si>
+  <si>
+    <t>Este servicio debe permitir consultar los hijos que dispone un padre</t>
+  </si>
+  <si>
+    <t>consultarPadres</t>
+  </si>
+  <si>
+    <t>Este servicio debe permitir consultar todos los padres que esten registrados en el sistema</t>
+  </si>
+  <si>
+    <t>consultarPago</t>
+  </si>
+  <si>
+    <t>Este serviico debe permitir consultar los pagos realizados por un numero de identificacion</t>
+  </si>
+  <si>
+    <t>actualizarHijo</t>
+  </si>
+  <si>
+    <t>Este servicio debe permitir la actualizacion de los datos del hijo de un padre.</t>
+  </si>
+  <si>
+    <t>consultarPedido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Este servicio debe permitir consultar </t>
   </si>
 </sst>
 </file>
@@ -407,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D13"/>
+  <dimension ref="A3:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -500,19 +542,60 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
+      <c r="A9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
+      <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
+      <c r="A12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
+      <c r="A13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>